<commit_message>
added asterisk so that excited delirium # correct
</commit_message>
<xml_diff>
--- a/db/Deaths in Police Custody full list.xlsx
+++ b/db/Deaths in Police Custody full list.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="2880" windowWidth="25360" windowHeight="15380" tabRatio="500"/>
+    <workbookView xWindow="1680" yWindow="120" windowWidth="25360" windowHeight="15380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2758" uniqueCount="2629">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2758" uniqueCount="2631">
   <si>
     <t>Lamont Morton</t>
   </si>
@@ -8052,13 +8052,19 @@
   <si>
     <t>law_weapons</t>
   </si>
+  <si>
+    <t>Homicide by law enforcement*</t>
+  </si>
+  <si>
+    <t>Unknown*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -8185,19 +8191,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -8542,9 +8548,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N145" sqref="N145"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q136" sqref="Q136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -17601,7 +17607,7 @@
         <v>2063</v>
       </c>
       <c r="R131" s="31" t="s">
-        <v>379</v>
+        <v>2630</v>
       </c>
       <c r="S131" s="4" t="s">
         <v>2064</v>
@@ -18390,7 +18396,7 @@
         <v>2458</v>
       </c>
       <c r="R142" s="31" t="s">
-        <v>11</v>
+        <v>2629</v>
       </c>
       <c r="S142" s="4" t="s">
         <v>2459</v>

</xml_diff>